<commit_message>
Update Linear Experiments and write that in thesis
</commit_message>
<xml_diff>
--- a/experiment/linear/ex9_1_10/compare/Alpha-Zero/ex9_1_10_Alpha-Zero.xlsx
+++ b/experiment/linear/ex9_1_10/compare/Alpha-Zero/ex9_1_10_Alpha-Zero.xlsx
@@ -494,13 +494,13 @@
         <v>-239.99999999999997</v>
       </c>
       <c r="E2">
-        <v>0.00024012</v>
+        <v>0.00036019</v>
       </c>
       <c r="F2">
-        <v>0.01547694</v>
+        <v>0.022946815</v>
       </c>
       <c r="G2">
-        <v>0.00041535998999999997</v>
+        <v>0.0005916887039552061</v>
       </c>
       <c r="H2">
         <v>1747</v>
@@ -535,13 +535,13 @@
         <v>-4.8528604996887255e20</v>
       </c>
       <c r="E3">
-        <v>0.06646275</v>
+        <v>0.091220866</v>
       </c>
       <c r="F3">
-        <v>0.08564985</v>
+        <v>0.105217551</v>
       </c>
       <c r="G3">
-        <v>0.07425232411764705</v>
+        <v>0.09548243956603773</v>
       </c>
       <c r="H3">
         <v>37881</v>

</xml_diff>